<commit_message>
validación de Tarea 1
</commit_message>
<xml_diff>
--- a/Integrantes.xlsx
+++ b/Integrantes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
@@ -31,20 +31,64 @@
     <t>17428518-7</t>
   </si>
   <si>
-    <t>Luis Miguel Jesus</t>
+    <t>17417030-4</t>
+  </si>
+  <si>
+    <t>Rojas Arias</t>
+  </si>
+  <si>
+    <t>Rojas</t>
+  </si>
+  <si>
+    <t>Luis Miguel</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>lmleon@outlook.com</t>
+  </si>
+  <si>
+    <t>b.rojas@icci.cl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,13 +108,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -87,12 +137,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Nombre"/>
     <tableColumn id="2" name="Apellido"/>
     <tableColumn id="4" name="Run"/>
+    <tableColumn id="3" name="Correo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -385,19 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,22 +459,50 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>